<commit_message>
daily work - add more info
</commit_message>
<xml_diff>
--- a/2018-ST市场记录.xlsx
+++ b/2018-ST市场记录.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ray/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ray/git/helloworld/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>日期</t>
     <rPh sb="0" eb="1">
@@ -149,11 +149,225 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>1.国际原油大幅走低</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">1.美参院以压倒性票数通过提案，限制特朗普关税权力. 2. </t>
+    <t xml:space="preserve">1.国际原油大幅走低. </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>高送转、机场航运、白酒</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>人民币贬值、水利水电、富勒烯，纺织、环保</t>
+    <rPh sb="0" eb="1">
+      <t>ren'mi'bi</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>bian'zhi</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>shui'li</t>
+    </rPh>
+    <rPh sb="8" eb="9">
+      <t>shui'dian</t>
+    </rPh>
+    <rPh sb="11" eb="12">
+      <t>fu'le'xi</t>
+    </rPh>
+    <rPh sb="15" eb="16">
+      <t>fang'zhi</t>
+    </rPh>
+    <rPh sb="18" eb="19">
+      <t>huan'bao</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 人民币贬值跌破6.74。 2.央行连续释放流动性</t>
+    <rPh sb="3" eb="4">
+      <t>ren'min'bi</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>bian'zhi</t>
+    </rPh>
+    <rPh sb="8" eb="9">
+      <t>die'po</t>
+    </rPh>
+    <rPh sb="18" eb="19">
+      <t>yang'hang</t>
+    </rPh>
+    <rPh sb="20" eb="21">
+      <t>lian'xu</t>
+    </rPh>
+    <rPh sb="22" eb="23">
+      <t>shi'fang</t>
+    </rPh>
+    <rPh sb="24" eb="25">
+      <t>liu'dong'xing</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.美参院以压倒性票数通过提案，限制特朗普关税权力. 2. 美国商务部和中兴达成协议取消制裁</t>
+    <rPh sb="30" eb="31">
+      <t>mei'guo</t>
+    </rPh>
+    <rPh sb="32" eb="33">
+      <t>shang'wu'b</t>
+    </rPh>
+    <rPh sb="35" eb="36">
+      <t>he</t>
+    </rPh>
+    <rPh sb="36" eb="37">
+      <t>zhong'xing</t>
+    </rPh>
+    <rPh sb="38" eb="39">
+      <t>da'cheng</t>
+    </rPh>
+    <rPh sb="40" eb="41">
+      <t>xie'yi</t>
+    </rPh>
+    <rPh sb="42" eb="43">
+      <t>qu'xiao'zhi'c</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5G、芯片、半导体、乡村振新</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.美方昨晚公布了对2000亿美元中国输美产品征收10%关税的建议产品清单</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>知识产权保护、网络安全、共享单车</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>特斯拉概念、农业</t>
+    <rPh sb="0" eb="1">
+      <t>te's'l</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>gai'n</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>nong'ye</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>中报业绩预增</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>种植业、电子竞技、小程序</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>高送转、次新股、石油矿业，天然气</t>
+    <rPh sb="13" eb="14">
+      <t>tian'ran'qi</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.天然气涨价</t>
+    <rPh sb="2" eb="3">
+      <t>tian'ran'qi</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>zhang'jia</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>医药，石油采掘，次新</t>
+    <rPh sb="0" eb="1">
+      <t>yi'yao</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>shi'you</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>cai'jue</t>
+    </rPh>
+    <rPh sb="8" eb="9">
+      <t>ci'xin</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 监管层表态维稳。2. 油价上涨</t>
+    <rPh sb="3" eb="4">
+      <t>jian'guan'c</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>biao'tai</t>
+    </rPh>
+    <rPh sb="8" eb="9">
+      <t>wei'wen</t>
+    </rPh>
+    <rPh sb="14" eb="15">
+      <t>you'jia'shang'zhang</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>次新，乡村振新，高送转，芯片</t>
+    <rPh sb="0" eb="1">
+      <t>ci'in</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>xiang'c</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>zhen'xin</t>
+    </rPh>
+    <rPh sb="8" eb="9">
+      <t>gao'song'z</t>
+    </rPh>
+    <rPh sb="12" eb="13">
+      <t>xin'p</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.美国加征关税消息落地。2. 有机硅价格上涨。3. 猪价上涨</t>
+    <rPh sb="2" eb="3">
+      <t>mei'guo</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>jia'zheng'guan's</t>
+    </rPh>
+    <rPh sb="8" eb="9">
+      <t>xiao'xi</t>
+    </rPh>
+    <rPh sb="10" eb="11">
+      <t>luo'di</t>
+    </rPh>
+    <rPh sb="16" eb="17">
+      <t>you'ji'gui</t>
+    </rPh>
+    <rPh sb="19" eb="20">
+      <t>jia'ge</t>
+    </rPh>
+    <rPh sb="21" eb="22">
+      <t>shang'z</t>
+    </rPh>
+    <rPh sb="27" eb="28">
+      <t>zhu'rou</t>
+    </rPh>
+    <rPh sb="28" eb="29">
+      <t>jia'ge</t>
+    </rPh>
+    <rPh sb="29" eb="30">
+      <t>shang'z</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>#1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -161,7 +375,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -177,13 +391,36 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="DengXian"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="0"/>
+      <name val="DengXian"/>
+      <family val="4"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -198,10 +435,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -479,14 +718,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="44.5" customWidth="1"/>
     <col min="4" max="4" width="36.33203125" customWidth="1"/>
     <col min="5" max="5" width="55.1640625" customWidth="1"/>
@@ -494,94 +735,213 @@
     <col min="7" max="7" width="29.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
+    <row r="2" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+      <c r="A2" s="1"/>
+      <c r="B2" s="2">
+        <v>-3.8999999999999998E-3</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+    </row>
+    <row r="3" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+      <c r="A3" s="3">
         <v>43298</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B3" s="2">
         <v>-5.7000000000000002E-3</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E3" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+      <c r="A4" s="3">
         <v>43297</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B4" s="2">
         <v>-6.1000000000000004E-3</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F4" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="1"/>
-      <c r="B4" s="2"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="1">
+      <c r="G4" s="1"/>
+    </row>
+    <row r="5" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+      <c r="A5" s="3"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+    </row>
+    <row r="6" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+      <c r="A6" s="3">
         <v>43294</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B6" s="2">
         <v>2.3E-3</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D6" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="1">
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+    </row>
+    <row r="7" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+      <c r="A7" s="3">
         <v>43293</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B7" s="2">
         <v>2.1600000000000001E-2</v>
       </c>
-      <c r="E6" t="s">
-        <v>16</v>
-      </c>
+      <c r="C7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+    </row>
+    <row r="8" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+      <c r="A8" s="3">
+        <v>43292</v>
+      </c>
+      <c r="B8" s="2">
+        <v>-1.7600000000000001E-2</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+    </row>
+    <row r="9" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+      <c r="A9" s="3">
+        <v>43291</v>
+      </c>
+      <c r="B9" s="2">
+        <v>4.4000000000000003E-3</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+      <c r="A10" s="3">
+        <v>43290</v>
+      </c>
+      <c r="B10" s="2">
+        <v>2.47E-2</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+    </row>
+    <row r="11" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+      <c r="A11" s="3"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+    </row>
+    <row r="12" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+      <c r="A12" s="3">
+        <v>43287</v>
+      </c>
+      <c r="B12" s="2">
+        <v>4.8999999999999998E-3</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G12" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>